<commit_message>
format Excel : Font và Border bảng
</commit_message>
<xml_diff>
--- a/ApartmentManagement/src/main/resources/com/utc2/apartmentmanagement/PDF_File/DoanhThuTheoThang.xlsx
+++ b/ApartmentManagement/src/main/resources/com/utc2/apartmentmanagement/PDF_File/DoanhThuTheoThang.xlsx
@@ -40,7 +40,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
@@ -49,7 +49,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="Times New Roman"/>
+      <sz val="16.0"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
       <sz val="16.0"/>
       <b val="true"/>
     </font>
@@ -62,7 +66,7 @@
       <patternFill patternType="darkGray"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -70,15 +74,35 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true"/>
   </cellXfs>
 </styleSheet>
 </file>
@@ -96,7 +120,10 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="1400">
+                <a:latin typeface="Times New Roman"/>
+                <a:cs typeface="Times New Roman"/>
+              </a:rPr>
               <a:t>Doanh thu theo tháng</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" sz="1100"/>
@@ -230,7 +257,7 @@
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="tr"/>
+      <c:legendPos val="b"/>
       <c:overlay val="false"/>
     </c:legend>
     <c:plotVisOnly val="true"/>
@@ -290,7 +317,7 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="s" s="1">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
       <c r="B1" s="0"/>
@@ -324,42 +351,42 @@
       <c r="N2" s="0"/>
     </row>
     <row r="13">
-      <c r="A13" t="s" s="0">
+      <c r="A13" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="B13" t="s" s="0">
+      <c r="B13" t="s" s="3">
         <v>2</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="n" s="0">
+      <c r="A14" t="n" s="3">
         <v>2.39E7</v>
       </c>
-      <c r="B14" t="s" s="0">
+      <c r="B14" t="s" s="3">
         <v>3</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="n" s="0">
+      <c r="A15" t="n" s="3">
         <v>1.214E7</v>
       </c>
-      <c r="B15" t="s" s="0">
+      <c r="B15" t="s" s="3">
         <v>4</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="n" s="0">
+      <c r="A16" t="n" s="3">
         <v>1.226E7</v>
       </c>
-      <c r="B16" t="s" s="0">
+      <c r="B16" t="s" s="3">
         <v>5</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="n" s="0">
+      <c r="A17" t="n" s="3">
         <v>1.247E7</v>
       </c>
-      <c r="B17" t="s" s="0">
+      <c r="B17" t="s" s="3">
         <v>6</v>
       </c>
     </row>

</xml_diff>